<commit_message>
Xong automation Thêm thuốc cho Bệnh nhân
</commit_message>
<xml_diff>
--- a/AutomationTest/TestCase/ThemSoLuongThuocCu/TestCaseTemp.xlsx
+++ b/AutomationTest/TestCase/ThemSoLuongThuocCu/TestCaseTemp.xlsx
@@ -15,7 +15,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="162913" fullCalcOnLoad="1" fullPrecision="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,26 +25,29 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+  <si>
+    <t>Medication</t>
+  </si>
+  <si>
+    <t>Quantity</t>
+  </si>
+  <si>
+    <t>Expected Result</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
   <si>
     <t>Panadol</t>
   </si>
   <si>
-    <t>Medication</t>
-  </si>
-  <si>
-    <t>Quantity</t>
-  </si>
-  <si>
-    <t>Result</t>
-  </si>
-  <si>
-    <t>Expected Result</t>
-  </si>
-  <si>
     <t>Lưu thành công</t>
   </si>
   <si>
+    <t>T</t>
+  </si>
+  <si>
     <t>Số lượng không hợp lệ</t>
   </si>
   <si>
@@ -57,14 +60,21 @@
     <t>Pass</t>
   </si>
   <si>
+    <t>6</t>
+  </si>
+  <si>
     <t>Fail</t>
+  </si>
+  <si>
+    <t>0</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -103,13 +113,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" applyFont="1" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -405,23 +415,23 @@
     <col min="3" max="3" width="28.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2">
       <c r="A2" s="2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" s="2">
         <v>3</v>
@@ -429,10 +439,13 @@
       <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D2" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3">
       <c r="A3" s="2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B3" s="2">
         <v>1</v>
@@ -440,130 +453,150 @@
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D3" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4">
       <c r="A4" s="2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B4" s="2">
         <v>-1</v>
       </c>
       <c r="C4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="0" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5">
       <c r="A5" s="2"/>
       <c r="B5" s="2">
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6">
       <c r="A6" s="2"/>
       <c r="B6" s="2">
         <v>1</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="D6" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
       <c r="A7" s="2"/>
       <c r="B7" s="2">
         <v>-1</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="D7" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9">
       <c r="A9" s="3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B9" s="2">
         <v>6</v>
       </c>
       <c r="C9" s="2"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10">
       <c r="A10" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" s="2"/>
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>11</v>
+      </c>
       <c r="C10" s="2"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11">
       <c r="A11" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" s="2"/>
+        <v>12</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="C11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13">
       <c r="A13" s="2"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15">
       <c r="A15" s="2"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17">
       <c r="A17" s="2"/>
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18">
       <c r="A18" s="2"/>
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19">
       <c r="A19" s="2"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20">
       <c r="A20" s="2"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21">
       <c r="A21" s="2"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22">
       <c r="A22" s="2"/>
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>